<commit_message>
feat(scrape): Implement scrape hoepli.it
</commit_message>
<xml_diff>
--- a/tests/data/test_dataframes/database.xlsx
+++ b/tests/data/test_dataframes/database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">isbn</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">feltrinelli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoepli</t>
   </si>
   <si>
     <t xml:space="preserve">ibs</t>
@@ -215,9 +218,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:P2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:P2"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:Q2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:Q2"/>
+  <tableColumns count="17">
     <tableColumn id="1" name="isbn"/>
     <tableColumn id="2" name="author"/>
     <tableColumn id="3" name="title"/>
@@ -228,12 +231,13 @@
     <tableColumn id="8" name="adelphi"/>
     <tableColumn id="9" name="buecher"/>
     <tableColumn id="10" name="feltrinelli"/>
-    <tableColumn id="11" name="ibs"/>
-    <tableColumn id="12" name="libcoop"/>
-    <tableColumn id="13" name="libraccio"/>
-    <tableColumn id="14" name="libuni"/>
-    <tableColumn id="15" name="mondadori"/>
-    <tableColumn id="16" name="osiander"/>
+    <tableColumn id="11" name="hoepli"/>
+    <tableColumn id="12" name="ibs"/>
+    <tableColumn id="13" name="libcoop"/>
+    <tableColumn id="14" name="libraccio"/>
+    <tableColumn id="15" name="libuni"/>
+    <tableColumn id="16" name="mondadori"/>
+    <tableColumn id="17" name="osiander"/>
   </tableColumns>
 </table>
 </file>
@@ -243,13 +247,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -300,25 +304,28 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>7.95</v>
@@ -328,7 +335,7 @@
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -336,14 +343,15 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
-        <v>23</v>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.buecher.de/artikel/buch/das-kapital/25646129/"/>
-    <hyperlink ref="P2" r:id="rId2" display="https://www.osiander.de/shop/home/artikeldetails/A1006759980"/>
+    <hyperlink ref="Q2" r:id="rId2" display="https://www.osiander.de/shop/home/artikeldetails/A1006759980"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>